<commit_message>
#4 importador excel modificado para fechas (manuales) de factura en Peaje y actualizaciones
</commit_message>
<xml_diff>
--- a/reportes/plantillaExcelFactura.xlsx
+++ b/reportes/plantillaExcelFactura.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="54">
-  <si>
-    <t>item</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="53">
   <si>
     <t>razon social</t>
   </si>
@@ -174,10 +171,10 @@
     <t>CODIGO-444</t>
   </si>
   <si>
+    <t>Producto Codigo</t>
+  </si>
+  <si>
     <t>nro</t>
-  </si>
-  <si>
-    <t>Producto Codigo</t>
   </si>
 </sst>
 </file>
@@ -185,7 +182,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -374,9 +371,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -384,13 +381,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -414,10 +411,10 @@
     <xf numFmtId="4" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -427,19 +424,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -448,7 +439,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -461,6 +452,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -509,7 +503,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -544,7 +538,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -756,7 +750,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -773,78 +767,75 @@
     <col min="13" max="13" width="19.5703125" customWidth="1"/>
     <col min="14" max="14" width="16.7109375" customWidth="1"/>
     <col min="15" max="15" width="24.42578125" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" customWidth="1"/>
-    <col min="17" max="17" width="27.140625" customWidth="1"/>
+    <col min="16" max="16" width="36.42578125" customWidth="1"/>
+    <col min="17" max="17" width="45.140625" customWidth="1"/>
     <col min="18" max="18" width="38.42578125" customWidth="1"/>
-    <col min="25" max="25" width="4.7109375" customWidth="1"/>
+    <col min="25" max="25" width="56.85546875" customWidth="1"/>
     <col min="26" max="26" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="16" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="Q1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z1" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26">
+      <c r="Y1" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="10">
         <v>1022915024</v>
@@ -853,16 +844,16 @@
         <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="13">
         <v>29.73</v>
       </c>
-      <c r="I2" s="25"/>
+      <c r="I2" s="23"/>
       <c r="J2" s="14">
         <v>29.73</v>
       </c>
@@ -872,32 +863,27 @@
       <c r="L2" s="8">
         <v>96115</v>
       </c>
-      <c r="M2" s="8">
-        <v>558</v>
-      </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="15">
-        <v>43373</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z2" s="23" t="s">
+      <c r="M2" s="9"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:26">
+      <c r="Y2" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="10">
         <v>4465363</v>
@@ -906,10 +892,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3" s="12">
         <v>1</v>
@@ -929,32 +915,27 @@
       <c r="L3" s="8">
         <v>96115</v>
       </c>
-      <c r="M3" s="8">
-        <v>559</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="15">
-        <v>43373</v>
-      </c>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z3" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26">
+      <c r="M3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y3" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="10">
         <v>4426064</v>
@@ -963,10 +944,10 @@
         <v>1</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" s="12">
         <v>1</v>
@@ -986,34 +967,29 @@
       <c r="L4" s="8">
         <v>96115</v>
       </c>
-      <c r="M4" s="8">
-        <v>560</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O4" s="15">
-        <v>43373</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q4" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z4" s="23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26">
+      <c r="M4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="15"/>
+      <c r="O4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10">
         <v>4421208</v>
@@ -1022,10 +998,10 @@
         <v>1</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" s="12">
         <v>1</v>
@@ -1043,34 +1019,29 @@
         <v>33120000</v>
       </c>
       <c r="L5" s="8"/>
-      <c r="M5" s="20">
-        <v>561</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O5" s="15">
-        <v>43373</v>
+      <c r="M5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="15"/>
+      <c r="O5" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q5" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z5" s="23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y5" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="10">
         <v>4382889</v>
@@ -1079,10 +1050,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" s="12">
         <v>1</v>
@@ -1102,34 +1073,29 @@
       <c r="L6" s="8">
         <v>96115</v>
       </c>
-      <c r="M6" s="8">
-        <v>562</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6" s="15">
-        <v>43373</v>
-      </c>
-      <c r="P6" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q6" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="R6" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z6" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26">
+      <c r="M6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="15"/>
+      <c r="O6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y6" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="10">
         <v>4423061</v>
@@ -1139,7 +1105,7 @@
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G7" s="12">
         <v>1</v>
@@ -1159,34 +1125,29 @@
       <c r="L7" s="8">
         <v>96115</v>
       </c>
-      <c r="M7" s="8">
-        <v>563</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O7" s="15">
-        <v>43373</v>
+      <c r="M7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="15"/>
+      <c r="O7" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q7" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R7" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z7" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26">
+        <v>29</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y7" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="10">
         <v>5906683</v>
@@ -1195,10 +1156,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" s="12">
         <v>1</v>
@@ -1218,34 +1179,29 @@
       <c r="L8" s="8">
         <v>96115</v>
       </c>
-      <c r="M8" s="8">
-        <v>564</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O8" s="15">
-        <v>43373</v>
+      <c r="M8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" s="15"/>
+      <c r="O8" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R8" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z8" s="23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
+        <v>29</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y8" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="10">
         <v>3773865</v>
@@ -1254,10 +1210,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9" s="12">
         <v>1</v>
@@ -1277,34 +1233,29 @@
       <c r="L9" s="8">
         <v>96115</v>
       </c>
-      <c r="M9" s="21">
-        <v>565</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O9" s="15">
-        <v>43373</v>
-      </c>
-      <c r="P9" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q9" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="R9" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z9" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26">
+      <c r="M9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="15"/>
+      <c r="O9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y9" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="10">
         <v>5162753</v>
@@ -1313,10 +1264,10 @@
         <v>1</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="12">
         <v>1</v>
@@ -1336,34 +1287,29 @@
       <c r="L10" s="8">
         <v>96115</v>
       </c>
-      <c r="M10" s="8">
-        <v>566</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O10" s="15">
-        <v>43373</v>
+      <c r="M10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" s="15"/>
+      <c r="O10" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R10" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z10" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26">
+        <v>29</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y10" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="10">
         <v>353599927</v>
@@ -1372,10 +1318,10 @@
         <v>1</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="12">
         <v>1</v>
@@ -1395,34 +1341,29 @@
       <c r="L11" s="8">
         <v>96115</v>
       </c>
-      <c r="M11" s="8">
-        <v>567</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O11" s="15">
-        <v>43373</v>
-      </c>
-      <c r="P11" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q11" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="R11" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z11" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26">
+      <c r="M11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" s="15"/>
+      <c r="O11" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P11" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y11" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="10">
         <v>3073696</v>
@@ -1431,10 +1372,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" s="12">
         <v>1</v>
@@ -1454,29 +1395,26 @@
       <c r="L12" s="8">
         <v>96115</v>
       </c>
-      <c r="M12" s="8">
-        <v>568</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O12" s="15"/>
+      <c r="M12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="15"/>
+      <c r="O12" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="P12" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q12" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R12" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
+        <v>29</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="10">
         <v>3536278</v>
@@ -1485,15 +1423,15 @@
         <v>1</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G13" s="12">
         <v>1</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="20">
         <v>10</v>
       </c>
       <c r="I13" s="14">
@@ -1508,31 +1446,26 @@
       <c r="L13" s="8">
         <v>96115</v>
       </c>
-      <c r="M13" s="8">
-        <v>569</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O13" s="15">
-        <v>43373</v>
+      <c r="M13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="15"/>
+      <c r="O13" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="P13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q13" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R13" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26">
+        <v>29</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
       <c r="A14" s="8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="10">
         <v>3536278</v>
@@ -1541,10 +1474,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="12">
         <v>1</v>
@@ -1564,34 +1497,29 @@
       <c r="L14" s="8">
         <v>96115</v>
       </c>
-      <c r="M14" s="8">
-        <v>569</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="O14" s="15">
-        <v>43373</v>
-      </c>
-      <c r="P14" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q14" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="R14" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z14" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
+      <c r="M14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" s="15"/>
+      <c r="O14" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P14" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q14" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y14" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
       <c r="A15" s="8">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="10">
         <v>3536278</v>
@@ -1600,10 +1528,10 @@
         <v>1</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G15" s="12">
         <v>1</v>
@@ -1623,34 +1551,29 @@
       <c r="L15" s="8">
         <v>96115</v>
       </c>
-      <c r="M15" s="8">
-        <v>569</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="O15" s="15">
-        <v>43373</v>
+      <c r="M15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N15" s="15"/>
+      <c r="O15" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="P15" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q15" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R15" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z15" s="23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26">
+        <v>29</v>
+      </c>
+      <c r="Q15" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y15" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
       <c r="A16" s="8">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="10">
         <v>3536278</v>
@@ -1659,10 +1582,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G16" s="12">
         <v>1</v>
@@ -1682,34 +1605,29 @@
       <c r="L16" s="8">
         <v>96115</v>
       </c>
-      <c r="M16" s="8">
-        <v>569</v>
-      </c>
-      <c r="N16" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O16" s="15">
-        <v>43373</v>
+      <c r="M16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="15"/>
+      <c r="O16" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="P16" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q16" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R16" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z16" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="Q16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y16" s="21" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:26">
       <c r="A17" s="8">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="10">
         <v>3536278</v>
@@ -1718,10 +1636,10 @@
         <v>1</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17" s="12">
         <v>1</v>
@@ -1741,38 +1659,33 @@
       <c r="L17" s="8">
         <v>96115</v>
       </c>
-      <c r="M17" s="8">
-        <v>569</v>
-      </c>
-      <c r="N17" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="O17" s="15">
-        <v>43373</v>
+      <c r="M17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17" s="15"/>
+      <c r="O17" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="P17" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q17" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R17" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z17" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q17" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y17" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="Y18" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
-      <c r="Z18" s="23" t="s">
-        <v>49</v>
-      </c>
-    </row>
     <row r="20" spans="1:26">
-      <c r="Z20" s="24"/>
+      <c r="Z20" s="22"/>
     </row>
     <row r="22" spans="1:26">
-      <c r="Z22" s="24"/>
+      <c r="Z22" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>